<commit_message>
completed the vote validation module
</commit_message>
<xml_diff>
--- a/modules/faster_rcnn_files/class_summary_df.xlsx
+++ b/modules/faster_rcnn_files/class_summary_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,10 +486,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
@@ -506,22 +506,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9099099099099099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -534,22 +534,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="H4" t="n">
-        <v>0.825</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -562,22 +562,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9369369369369369</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -590,22 +590,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="7">
@@ -618,22 +618,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8058252427184466</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -646,22 +646,20 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F8" t="n">
-        <v>116</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>0.9137931034482759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -674,22 +672,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8899082568807339</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -702,22 +700,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>122</v>
+        <v>21</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="H10" t="n">
-        <v>0.8934426229508197</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -730,22 +728,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9805825242718447</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -758,22 +756,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="G12" t="n">
         <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9320388349514563</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -786,22 +784,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -814,22 +812,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="H14" t="n">
-        <v>0.8538461538461538</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -842,22 +840,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>0.963963963963964</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -866,26 +864,26 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>key</t>
+          <t>invalid_stamp</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="H16" t="n">
-        <v>0.9279279279279279</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -894,26 +892,26 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ladder</t>
+          <t>key</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="G17" t="n">
         <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0.9357798165137615</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -922,26 +920,26 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>ladder</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="H18" t="n">
-        <v>0.9719626168224299</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -950,26 +948,26 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>lotus</t>
+          <t>lock</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="G19" t="n">
-        <v>1</v>
+        <v>0.8235294117647058</v>
       </c>
       <c r="H19" t="n">
-        <v>0.8557692307692307</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -978,26 +976,26 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>loud_speaker</t>
+          <t>lotus</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E20" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H20" t="n">
-        <v>0.7169811320754716</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1006,26 +1004,26 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>mother_and_child</t>
+          <t>loud_speaker</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="G21" t="n">
         <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>0.9145299145299145</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1034,11 +1032,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>namaste</t>
+          <t>mother_and_child</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -1047,13 +1045,13 @@
         <v>5</v>
       </c>
       <c r="F22" t="n">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="G22" t="n">
         <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="23">
@@ -1062,26 +1060,26 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>nepali_big_basket</t>
+          <t>namaste</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>115</v>
+        <v>14</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>0.8434782608695652</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1090,26 +1088,24 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>nepali_cap</t>
+          <t>nepali_big_basket</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F24" t="n">
-        <v>110</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>0.7636363636363637</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1118,26 +1114,26 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>nepali_jug</t>
+          <t>nepali_cap</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="H25" t="n">
-        <v>0.9664429530201343</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1146,26 +1142,26 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>nepali_madal</t>
+          <t>nepali_jug</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="G26" t="n">
         <v>1</v>
       </c>
       <c r="H26" t="n">
-        <v>0.8909090909090909</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1174,26 +1170,26 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>nepali_small_basket</t>
+          <t>nepali_madal</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="G27" t="n">
         <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>0.8125</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="28">
@@ -1202,26 +1198,26 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>owl</t>
+          <t>nepali_small_basket</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="G28" t="n">
         <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>0.7899159663865546</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1230,26 +1226,26 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>pen</t>
+          <t>owl</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>89</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F29" t="n">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="G29" t="n">
         <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>0.7946428571428571</v>
+        <v>0.07142857142857142</v>
       </c>
     </row>
     <row r="30">
@@ -1258,26 +1254,26 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>roaster</t>
+          <t>pen</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="G30" t="n">
         <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>0.9454545454545454</v>
+        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="31">
@@ -1286,26 +1282,26 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>sheep</t>
+          <t>roaster</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>0.8429752066115702</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1314,26 +1310,26 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>stamp</t>
+          <t>sheep</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>157</v>
+        <v>14</v>
       </c>
       <c r="G32" t="n">
         <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>0.9745222929936306</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1346,22 +1342,22 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="H33" t="n">
-        <v>0.9603960396039604</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1374,22 +1370,22 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>0.9122807017543859</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1402,22 +1398,22 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="G35" t="n">
         <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0.9428571428571428</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1430,22 +1426,22 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0.8125</v>
       </c>
       <c r="H36" t="n">
-        <v>0.9369369369369369</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1458,22 +1454,22 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="H37" t="n">
-        <v>0.9338842975206612</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1486,22 +1482,22 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>117</v>
+        <v>15</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="H38" t="n">
-        <v>0.8632478632478633</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1514,22 +1510,22 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="G39" t="n">
         <v>1</v>
       </c>
       <c r="H39" t="n">
-        <v>0.8050847457627118</v>
+        <v>0.9285714285714286</v>
       </c>
     </row>
     <row r="40">
@@ -1542,22 +1538,22 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>0.9357798165137615</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1566,26 +1562,26 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>water_glass</t>
+          <t>valid_stamp</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="G41" t="n">
         <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>0.8155339805825242</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1594,26 +1590,26 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>water_jug</t>
+          <t>water_glass</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D42" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="G42" t="n">
-        <v>0.8363636363636363</v>
+        <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>0.7666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1622,26 +1618,26 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>woman_man</t>
+          <t>water_jug</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="H43" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1650,26 +1646,54 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>woman_man</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>13</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>14</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>wooden_wheel</t>
         </is>
       </c>
-      <c r="C44" t="n">
-        <v>106</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="n">
-        <v>3</v>
-      </c>
-      <c r="F44" t="n">
-        <v>109</v>
-      </c>
-      <c r="G44" t="n">
-        <v>1</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0.9724770642201835</v>
+      <c r="C45" t="n">
+        <v>14</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>14</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ammended in the vote validation module. Worked in the balane dataset
</commit_message>
<xml_diff>
--- a/modules/faster_rcnn_files/class_summary_df.xlsx
+++ b/modules/faster_rcnn_files/class_summary_df.xlsx
@@ -483,15 +483,17 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
+        <v>47</v>
+      </c>
+      <c r="E2" t="n">
+        <v>99</v>
+      </c>
+      <c r="F2" t="n">
+        <v>146</v>
+      </c>
+      <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="n">
-        <v>14</v>
-      </c>
-      <c r="F2" t="n">
-        <v>14</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>0</v>
       </c>
@@ -506,22 +508,22 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>84</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" t="n">
         <v>14</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
       <c r="F3" t="n">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="4">
@@ -534,22 +536,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F4" t="n">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.7171717171717171</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0.7244897959183674</v>
       </c>
     </row>
     <row r="5">
@@ -562,22 +564,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="G5" t="n">
-        <v>0.875</v>
+        <v>0.9595959595959596</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>0.9595959595959596</v>
       </c>
     </row>
     <row r="6">
@@ -590,22 +592,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="7">
@@ -618,22 +620,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F7" t="n">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.8686868686868687</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>0.8686868686868687</v>
       </c>
     </row>
     <row r="8">
@@ -646,20 +648,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F8" t="n">
-        <v>14</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
+        <v>119</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.7474747474747475</v>
+      </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.7872340425531915</v>
       </c>
     </row>
     <row r="9">
@@ -672,22 +676,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="D9" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F9" t="n">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5384615384615384</v>
+        <v>0.8080808080808081</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0.8247422680412371</v>
       </c>
     </row>
     <row r="10">
@@ -700,22 +704,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.9494949494949495</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>0.9591836734693877</v>
       </c>
     </row>
     <row r="11">
@@ -728,19 +732,19 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="G11" t="n">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
@@ -756,22 +760,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F12" t="n">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0.8080808080808081</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>0.8247422680412371</v>
       </c>
     </row>
     <row r="13">
@@ -784,22 +788,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0.9393939393939394</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>0.9393939393939394</v>
       </c>
     </row>
     <row r="14">
@@ -812,22 +816,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F14" t="n">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.6565656565656566</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>0.6989247311827957</v>
       </c>
     </row>
     <row r="15">
@@ -840,22 +844,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0.9494949494949495</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>0.9494949494949495</v>
       </c>
     </row>
     <row r="16">
@@ -868,22 +872,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="G16" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>0.9411764705882353</v>
       </c>
     </row>
     <row r="17">
@@ -896,22 +900,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F17" t="n">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="18">
@@ -924,22 +928,22 @@
         </is>
       </c>
       <c r="C18" t="n">
+        <v>83</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="n">
         <v>14</v>
       </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
       <c r="F18" t="n">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="G18" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.8383838383838383</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0.8556701030927835</v>
       </c>
     </row>
     <row r="19">
@@ -952,22 +956,22 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F19" t="n">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="H19" t="n">
-        <v>1</v>
+        <v>0.865979381443299</v>
       </c>
     </row>
     <row r="20">
@@ -980,22 +984,22 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="D20" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.8686868686868687</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0.8958333333333334</v>
       </c>
     </row>
     <row r="21">
@@ -1008,22 +1012,22 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F21" t="n">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0.8080808080808081</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0.8080808080808081</v>
       </c>
     </row>
     <row r="22">
@@ -1036,22 +1040,22 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E22" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F22" t="n">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0.9191919191919192</v>
       </c>
       <c r="H22" t="n">
-        <v>0.6428571428571429</v>
+        <v>0.9285714285714286</v>
       </c>
     </row>
     <row r="23">
@@ -1064,22 +1068,22 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>0.9595959595959596</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>0.9595959595959596</v>
       </c>
     </row>
     <row r="24">
@@ -1092,20 +1096,22 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E24" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F24" t="n">
-        <v>14</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
+        <v>124</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>0.7252747252747253</v>
       </c>
     </row>
     <row r="25">
@@ -1118,22 +1124,22 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="D25" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F25" t="n">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5384615384615384</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>0.8279569892473119</v>
       </c>
     </row>
     <row r="26">
@@ -1146,22 +1152,22 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F26" t="n">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>0.826530612244898</v>
       </c>
     </row>
     <row r="27">
@@ -1174,22 +1180,22 @@
         </is>
       </c>
       <c r="C27" t="n">
+        <v>81</v>
+      </c>
+      <c r="D27" t="n">
+        <v>18</v>
+      </c>
+      <c r="E27" t="n">
         <v>12</v>
       </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>2</v>
-      </c>
       <c r="F27" t="n">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="H27" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8709677419354839</v>
       </c>
     </row>
     <row r="28">
@@ -1202,22 +1208,22 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F28" t="n">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="29">
@@ -1230,22 +1236,22 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E29" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F29" t="n">
-        <v>14</v>
+        <v>129</v>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>0.5656565656565656</v>
       </c>
       <c r="H29" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.6511627906976745</v>
       </c>
     </row>
     <row r="30">
@@ -1258,22 +1264,22 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F30" t="n">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="G30" t="n">
-        <v>1</v>
+        <v>0.7878787878787878</v>
       </c>
       <c r="H30" t="n">
-        <v>0.7857142857142857</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="31">
@@ -1286,22 +1292,22 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F31" t="n">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>0.9072164948453608</v>
       </c>
     </row>
     <row r="32">
@@ -1314,22 +1320,22 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>0.898989898989899</v>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>0.9270833333333334</v>
       </c>
     </row>
     <row r="33">
@@ -1342,22 +1348,22 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="G33" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.9696969696969697</v>
       </c>
       <c r="H33" t="n">
-        <v>1</v>
+        <v>0.9696969696969697</v>
       </c>
     </row>
     <row r="34">
@@ -1370,22 +1376,22 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F34" t="n">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>0.7578947368421053</v>
       </c>
     </row>
     <row r="35">
@@ -1398,22 +1404,22 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F35" t="n">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>0.9393939393939394</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>0.9489795918367347</v>
       </c>
     </row>
     <row r="36">
@@ -1426,22 +1432,22 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="D36" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F36" t="n">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="G36" t="n">
-        <v>0.8125</v>
+        <v>0.8282828282828283</v>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>0.8541666666666666</v>
       </c>
     </row>
     <row r="37">
@@ -1454,22 +1460,22 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F37" t="n">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="G37" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.8282828282828283</v>
       </c>
       <c r="H37" t="n">
-        <v>1</v>
+        <v>0.8817204301075269</v>
       </c>
     </row>
     <row r="38">
@@ -1482,22 +1488,22 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F38" t="n">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="G38" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.8282828282828283</v>
       </c>
       <c r="H38" t="n">
-        <v>1</v>
+        <v>0.8282828282828283</v>
       </c>
     </row>
     <row r="39">
@@ -1510,22 +1516,22 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F39" t="n">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>0.8383838383838383</v>
       </c>
       <c r="H39" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.8829787234042553</v>
       </c>
     </row>
     <row r="40">
@@ -1538,22 +1544,22 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F40" t="n">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>0.8484848484848485</v>
       </c>
     </row>
     <row r="41">
@@ -1566,22 +1572,22 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="H41" t="n">
-        <v>1</v>
+        <v>0.9583333333333334</v>
       </c>
     </row>
     <row r="42">
@@ -1594,22 +1600,22 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F42" t="n">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="G42" t="n">
-        <v>1</v>
+        <v>0.9494949494949495</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0.9494949494949495</v>
       </c>
     </row>
     <row r="43">
@@ -1622,22 +1628,22 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F43" t="n">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="G43" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.8080808080808081</v>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>0.8247422680412371</v>
       </c>
     </row>
     <row r="44">
@@ -1650,22 +1656,22 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="G44" t="n">
         <v>1</v>
       </c>
       <c r="H44" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1678,22 +1684,22 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="G45" t="n">
-        <v>1</v>
+        <v>0.9494949494949495</v>
       </c>
       <c r="H45" t="n">
-        <v>1</v>
+        <v>0.9494949494949495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>